<commit_message>
all step and stl files
</commit_message>
<xml_diff>
--- a/docs/hardware/Helmoro_BoM_electronics.xlsx
+++ b/docs/hardware/Helmoro_BoM_electronics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHE\Documents\Git_Data\HelMoRo\docs\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B325784D-5983-42B3-B53A-9C6118F0C8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D1D527-E77E-496D-9444-75EDAE19D4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -4774,7 +4774,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4845,7 +4845,7 @@
         <v>67</v>
       </c>
       <c r="F3" s="6">
-        <v>11.3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4885,7 +4885,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="6">
-        <v>71.3</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -5105,7 +5105,7 @@
         <v>59</v>
       </c>
       <c r="F16" s="6">
-        <v>5.15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -5125,7 +5125,7 @@
         <v>79</v>
       </c>
       <c r="F17" s="6">
-        <v>2.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
@@ -5205,7 +5205,7 @@
         <v>101</v>
       </c>
       <c r="F21" s="6">
-        <v>1.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -7553,7 +7553,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7C2E72-762D-4B92-9001-4D5CFCA7E876}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED80A6F9-A719-43C3-8C0D-B89A6F9CBB84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="HelblingDocs"/>

</xml_diff>